<commit_message>
plots and code update
</commit_message>
<xml_diff>
--- a/Data/Solutions/N5_1111-0000_DP_cpm_solution.xlsx
+++ b/Data/Solutions/N5_1111-0000_DP_cpm_solution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>Info</t>
   </si>
@@ -88,6 +88,39 @@
   </si>
   <si>
     <t>[1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>FEP 0.0625</t>
+  </si>
+  <si>
+    <t>CXM 2.25</t>
+  </si>
+  <si>
+    <t>AMC 8_8</t>
+  </si>
+  <si>
+    <t>ZOX 0.0156</t>
+  </si>
+  <si>
+    <t>CEC 4</t>
+  </si>
+  <si>
+    <t>CPR 16</t>
+  </si>
+  <si>
+    <t>AM 512</t>
+  </si>
+  <si>
+    <t>TZP 8_32</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>CPR 12</t>
+  </si>
+  <si>
+    <t>FEP 0.0312</t>
   </si>
 </sst>
 </file>
@@ -469,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>634.2</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -939,200 +972,200 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>23</v>
-      </c>
-      <c r="E5">
-        <v>23</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>19</v>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-      <c r="E11">
-        <v>7</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14">
-        <v>22</v>
-      </c>
-      <c r="E14">
-        <v>22</v>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16">
-        <v>16</v>
-      </c>
-      <c r="D16">
-        <v>16</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17">
-        <v>18</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>